<commit_message>
adição de html e JS contato
</commit_message>
<xml_diff>
--- a/Detalhamento Linkagem JS e HTML.xlsx
+++ b/Detalhamento Linkagem JS e HTML.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$X$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$AA$67</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -162,66 +162,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>81395</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>135082</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>392257</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1732</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Retângulo Arredondado 7"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27963668" y="1381991"/>
-          <a:ext cx="916998" cy="438150"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FA5F00"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1"/>
-            <a:t>Contato</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -466,8 +406,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12023146" y="7981951"/>
-          <a:ext cx="1623579" cy="5048249"/>
+          <a:off x="12269930" y="7973292"/>
+          <a:ext cx="1662545" cy="5048249"/>
           <a:chOff x="18697575" y="742950"/>
           <a:chExt cx="1632602" cy="5048249"/>
         </a:xfrm>
@@ -750,8 +690,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="219075" y="1297132"/>
-          <a:ext cx="3770168" cy="3152775"/>
+          <a:off x="219075" y="1288473"/>
+          <a:ext cx="3848100" cy="3152775"/>
           <a:chOff x="219075" y="742950"/>
           <a:chExt cx="3770168" cy="3152775"/>
         </a:xfrm>
@@ -1192,8 +1132,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4179743" y="1297131"/>
-          <a:ext cx="6787863" cy="6486525"/>
+          <a:off x="4257675" y="1288472"/>
+          <a:ext cx="6943726" cy="6486525"/>
           <a:chOff x="4200525" y="742949"/>
           <a:chExt cx="6829426" cy="6486525"/>
         </a:xfrm>
@@ -2264,7 +2204,6 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="ctr"/>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100" b="1">
                   <a:solidFill>
@@ -2274,7 +2213,22 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>#criarAcc - caixa</a:t>
+                <a:t>#criarAcc - </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="85000"/>
+                      <a:lumOff val="15000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>elem</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
@@ -2284,16 +2238,21 @@
                       <a:lumOff val="15000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                </a:rPr>
-                <a:t> de texto estado</a:t>
-              </a:r>
-              <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> a ser clicacado</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="85000"/>
                     <a:lumOff val="15000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst/>
               </a:endParaRPr>
             </a:p>
           </xdr:txBody>
@@ -2541,8 +2500,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11091430" y="1297133"/>
-          <a:ext cx="3173556" cy="2819400"/>
+          <a:off x="11325225" y="1288474"/>
+          <a:ext cx="3238500" cy="2819400"/>
           <a:chOff x="11153775" y="742951"/>
           <a:chExt cx="3190875" cy="2819400"/>
         </a:xfrm>
@@ -2603,7 +2562,14 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l"/>
-              <a:endParaRPr lang="pt-BR" sz="1100"/>
+              <a:endParaRPr lang="pt-BR" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -2646,7 +2612,11 @@
             <a:p>
               <a:pPr algn="ctr"/>
               <a:r>
-                <a:rPr lang="pt-BR" sz="1100" b="1"/>
+                <a:rPr lang="pt-BR" sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
                 <a:t>Login</a:t>
               </a:r>
             </a:p>
@@ -2926,7 +2896,6 @@
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="pt-BR" sz="1100" b="1">
                 <a:solidFill>
@@ -2936,7 +2905,22 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>#continuar - caixa</a:t>
+              <a:t>#continuar - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>elem</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
@@ -2946,16 +2930,21 @@
                     <a:lumOff val="15000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t> de texto estado</a:t>
+              <a:t> a ser clicacado</a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+            <a:endParaRPr lang="pt-BR">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="85000"/>
                   <a:lumOff val="15000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2983,8 +2972,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="214745" y="7981951"/>
-          <a:ext cx="5804189" cy="5048249"/>
+          <a:off x="214745" y="7973292"/>
+          <a:ext cx="5921087" cy="5048249"/>
           <a:chOff x="14478000" y="742950"/>
           <a:chExt cx="5838825" cy="5048249"/>
         </a:xfrm>
@@ -3452,7 +3441,6 @@
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="pt-BR" sz="1100" b="1">
                 <a:solidFill>
@@ -3462,10 +3450,10 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>#voltar - caixa</a:t>
+              <a:t>#</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="sng">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="85000"/>
@@ -3473,15 +3461,46 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t> de texto estado</a:t>
+              <a:t>voltar - </a:t>
             </a:r>
-            <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>id</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" u="sng" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> a ser clicado</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" u="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="85000"/>
                   <a:lumOff val="15000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -3509,8 +3528,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6133234" y="7981951"/>
-          <a:ext cx="5702877" cy="5048249"/>
+          <a:off x="6263120" y="7973292"/>
+          <a:ext cx="5819775" cy="5048249"/>
           <a:chOff x="20316825" y="742950"/>
           <a:chExt cx="5702877" cy="5048249"/>
         </a:xfrm>
@@ -4385,6 +4404,269 @@
                 </a:solidFill>
               </a:rPr>
               <a:t> do elemento clicada</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>542923</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12124</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="78" name="Agrupar 77"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="14801849" y="1288474"/>
+          <a:ext cx="1838324" cy="2819400"/>
+          <a:chOff x="11153775" y="742951"/>
+          <a:chExt cx="1807788" cy="2819400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="81" name="Agrupar 80"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="11153775" y="742951"/>
+            <a:ext cx="1807788" cy="2819400"/>
+            <a:chOff x="7686675" y="742951"/>
+            <a:chExt cx="1807788" cy="2819400"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="90" name="Retângulo Arredondado 89"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7686675" y="742951"/>
+              <a:ext cx="1807788" cy="2819400"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 4571"/>
+              </a:avLst>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="91" name="Retângulo Arredondado 90"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7734300" y="857250"/>
+              <a:ext cx="923925" cy="438150"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FA5F00"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="1"/>
+                <a:t>Contato</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="82" name="Retângulo Arredondado 81"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11399059" y="1333501"/>
+            <a:ext cx="1219975" cy="438150"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>voltaPagContato</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="88" name="Retângulo Arredondado 87"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11580035" y="1828800"/>
+            <a:ext cx="1276350" cy="504826"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>#contato - elem</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> a ser clicacado</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1100" b="1">
               <a:solidFill>
@@ -4671,13 +4953,14 @@
   </sheetPr>
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X68" sqref="A1:X68"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AV11" sqref="AV11:AV12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -4687,7 +4970,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>